<commit_message>
chore: add example weather data excel
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\weather-scraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\weather-scraping\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80E50A6-AF0E-4AC5-82F0-C704CA4BD615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C6AF15-723C-43BD-8280-21491CAE1EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15804" yWindow="2604" windowWidth="12960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>EXCEL_FILE_NAME</t>
   </si>
@@ -31,7 +31,10 @@
     <t>DATE_COLUMN_EXCEL_INDEX</t>
   </si>
   <si>
-    <t>temperaturi</t>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>weather_data</t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,13 +447,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
-        <v>2022</v>
-      </c>
       <c r="C2" s="4">
-        <v>184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>